<commit_message>
Fixes and experiments for letter approach
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
   <si>
     <t>Content</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>Some chatter by me, tokenized</t>
+  </si>
+  <si>
+    <t>Wessel1</t>
+  </si>
+  <si>
+    <t>All of Wessel's sent emails still available from SHARE</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Broken version of letter approach</t>
+  </si>
+  <si>
+    <t>Halverwege gestopt, is waarschijnlijk iets lager</t>
   </si>
 </sst>
 </file>
@@ -149,10 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -447,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -908,6 +924,87 @@
         <v>27</v>
       </c>
     </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>17</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22">
+        <v>13</v>
+      </c>
+      <c r="G22">
+        <v>22</v>
+      </c>
+      <c r="H22">
+        <v>390</v>
+      </c>
+      <c r="I22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <v>19</v>
+      </c>
+      <c r="G24">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -916,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -980,6 +1077,20 @@
         <v>4500</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -991,7 +1102,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
New experiments, fixed tweet collection script
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
   <si>
     <t>Content</t>
   </si>
@@ -120,7 +120,25 @@
     <t>Broken version of letter approach</t>
   </si>
   <si>
-    <t>Halverwege gestopt, is waarschijnlijk iets lager</t>
+    <t>Stop halfway</t>
+  </si>
+  <si>
+    <t>Implemented multicore testing</t>
+  </si>
+  <si>
+    <t>Same, but with ucto</t>
+  </si>
+  <si>
+    <t>Wessel1, Wessel1-lex, Sonar1, Sonar1-lex</t>
+  </si>
+  <si>
+    <t>Wessel1, Sonar1, Wessel1-lex, Sonar1-lex</t>
+  </si>
+  <si>
+    <t>Wessel1, Wessel1-lex</t>
+  </si>
+  <si>
+    <t>Sonar1, Sonar1-lex</t>
   </si>
 </sst>
 </file>
@@ -463,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,30 +997,291 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="3">
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3">
         <v>0.1</v>
       </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24">
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23">
         <v>19</v>
       </c>
-      <c r="G24">
+      <c r="G23">
         <v>25</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I23" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>77</v>
+      </c>
+      <c r="I25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <v>29</v>
+      </c>
+      <c r="H26">
+        <v>11579</v>
+      </c>
+      <c r="I26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>73</v>
+      </c>
+      <c r="I27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="G28">
+        <v>29</v>
+      </c>
+      <c r="H28">
+        <v>13760</v>
+      </c>
+      <c r="I28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>12</v>
+      </c>
+      <c r="H30">
+        <v>146</v>
+      </c>
+      <c r="I30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31">
+        <v>23</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>22508</v>
+      </c>
+      <c r="I31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32">
+        <v>23</v>
+      </c>
+      <c r="G32">
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <v>22292</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33">
+        <v>23</v>
+      </c>
+      <c r="G33">
+        <v>29</v>
+      </c>
+      <c r="H33">
+        <v>20800</v>
+      </c>
+      <c r="I33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>31446</v>
+      </c>
+      <c r="I34" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed formula for keys saved, did more experiments
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
   <si>
     <t>Content</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Sonar1, Sonar1-lex</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Basic set-up, but timblserver now and new calculation of cks and skks… but possibly too slow nl corpus</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1282,6 +1288,64 @@
       </c>
       <c r="I34" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36">
+        <v>15</v>
+      </c>
+      <c r="G36">
+        <v>20</v>
+      </c>
+      <c r="H36">
+        <v>13</v>
+      </c>
+      <c r="I36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37">
+        <v>33</v>
+      </c>
+      <c r="G37">
+        <v>41</v>
+      </c>
+      <c r="H37">
+        <v>2661</v>
+      </c>
+      <c r="I37" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored settings, added punctuation = accept
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="46">
   <si>
     <t>Content</t>
   </si>
@@ -144,7 +144,16 @@
     <t>Same</t>
   </si>
   <si>
-    <t>Basic set-up, but timblserver now and new calculation of cks and skks… but possibly too slow nl corpus</t>
+    <t>Basic set-up, but timblserver now and new calculation of cks and skks…</t>
+  </si>
+  <si>
+    <t>Switched safety net to the low-attenuation one</t>
+  </si>
+  <si>
+    <t>Same, notice low attenuation value now possible</t>
+  </si>
+  <si>
+    <t>Added punctuation = accept prediction</t>
   </si>
 </sst>
 </file>
@@ -487,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1346,6 +1355,148 @@
       </c>
       <c r="I37" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39">
+        <v>4500</v>
+      </c>
+      <c r="D39">
+        <v>4500</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39">
+        <v>15</v>
+      </c>
+      <c r="G39">
+        <v>20</v>
+      </c>
+      <c r="H39">
+        <v>20</v>
+      </c>
+      <c r="I39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40">
+        <v>20</v>
+      </c>
+      <c r="G40">
+        <v>24</v>
+      </c>
+      <c r="H40">
+        <v>20</v>
+      </c>
+      <c r="I40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42">
+        <v>21</v>
+      </c>
+      <c r="G42">
+        <v>23</v>
+      </c>
+      <c r="H42">
+        <v>13</v>
+      </c>
+      <c r="I42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43">
+        <v>33</v>
+      </c>
+      <c r="G43">
+        <v>41</v>
+      </c>
+      <c r="H43">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45">
+        <v>38</v>
+      </c>
+      <c r="G45">
+        <v>44</v>
+      </c>
+      <c r="H45">
+        <v>2696</v>
+      </c>
+      <c r="I45" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did some more experiments
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="8595" windowHeight="4680"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="8595" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="62">
   <si>
     <t>Content</t>
   </si>
@@ -175,6 +175,33 @@
   </si>
   <si>
     <t>Recency buffer 100, with words longer than 4 chars</t>
+  </si>
+  <si>
+    <t>Recency buffer 100, but only words longer than 3 chars are accepted in the buffer</t>
+  </si>
+  <si>
+    <t>Recency buffer 50, but only words longer than 3 chars are accepted in the buffer</t>
+  </si>
+  <si>
+    <t>Recency buffer 50, but only words longer than 5 chars are accepted in the buffer</t>
+  </si>
+  <si>
+    <t>Recency buffer 50 influences TiMBL</t>
+  </si>
+  <si>
+    <t>Recency buffer 100 influences TiMBL</t>
+  </si>
+  <si>
+    <t>Recency buffer 200 influences TiMBL</t>
+  </si>
+  <si>
+    <t>Recency buffer 50/100/200/300 only influences TiMBL for general model</t>
+  </si>
+  <si>
+    <t>Sonar2</t>
+  </si>
+  <si>
+    <t>Stuff from Wikipedia, blogs, emails, tweets, chats, sms, subtitles &amp; e-magazine</t>
   </si>
 </sst>
 </file>
@@ -517,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1807,6 +1834,209 @@
         <v>52</v>
       </c>
     </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60">
+        <v>36</v>
+      </c>
+      <c r="G60">
+        <v>41</v>
+      </c>
+      <c r="H60">
+        <v>1115</v>
+      </c>
+      <c r="I60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61">
+        <v>36</v>
+      </c>
+      <c r="G61">
+        <v>42</v>
+      </c>
+      <c r="H61">
+        <v>1127</v>
+      </c>
+      <c r="I61" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62">
+        <v>36</v>
+      </c>
+      <c r="G62">
+        <v>42</v>
+      </c>
+      <c r="H62">
+        <v>1098</v>
+      </c>
+      <c r="I62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64">
+        <v>38</v>
+      </c>
+      <c r="G64">
+        <v>44</v>
+      </c>
+      <c r="H64">
+        <v>1263</v>
+      </c>
+      <c r="I64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65">
+        <v>38</v>
+      </c>
+      <c r="G65">
+        <v>44</v>
+      </c>
+      <c r="H65">
+        <v>1280</v>
+      </c>
+      <c r="I65" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66">
+        <v>38</v>
+      </c>
+      <c r="G66">
+        <v>44</v>
+      </c>
+      <c r="H66">
+        <v>1256</v>
+      </c>
+      <c r="I66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67">
+        <v>39</v>
+      </c>
+      <c r="G67">
+        <v>45</v>
+      </c>
+      <c r="H67">
+        <v>1037</v>
+      </c>
+      <c r="I67" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1815,10 +2045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1876,7 +2106,7 @@
         <v>90</v>
       </c>
       <c r="D4">
-        <v>4500</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1891,6 +2121,17 @@
       </c>
       <c r="D5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote main part of paper, did more experiments
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="8595" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests" sheetId="2" r:id="rId1"/>
-    <sheet name="Training dirs" sheetId="1" r:id="rId2"/>
-    <sheet name="Testfiles" sheetId="3" r:id="rId3"/>
+    <sheet name="General tests" sheetId="2" r:id="rId1"/>
+    <sheet name="Twitter tests" sheetId="4" r:id="rId2"/>
+    <sheet name="Training dirs" sheetId="1" r:id="rId3"/>
+    <sheet name="Testfiles" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="124">
   <si>
     <t>Content</t>
   </si>
@@ -202,6 +203,192 @@
   </si>
   <si>
     <t>Stuff from Wikipedia, blogs, emails, tweets, chats, sms, subtitles &amp; e-magazine</t>
+  </si>
+  <si>
+    <t>Tweeter</t>
+  </si>
+  <si>
+    <t>Nr words</t>
+  </si>
+  <si>
+    <t>SKSS PERS</t>
+  </si>
+  <si>
+    <t>CKS PERS</t>
+  </si>
+  <si>
+    <t>CKS NL</t>
+  </si>
+  <si>
+    <t>SKSS NL</t>
+  </si>
+  <si>
+    <t>artbysophia</t>
+  </si>
+  <si>
+    <t>baspaternotte</t>
+  </si>
+  <si>
+    <t>marktwain2</t>
+  </si>
+  <si>
+    <t>pinaatje</t>
+  </si>
+  <si>
+    <t>pienbetuwe</t>
+  </si>
+  <si>
+    <t>rider_ot_storm</t>
+  </si>
+  <si>
+    <t>mrsmartine</t>
+  </si>
+  <si>
+    <t>chrisklomp</t>
+  </si>
+  <si>
+    <t>leolewin</t>
+  </si>
+  <si>
+    <t>contentgirl</t>
+  </si>
+  <si>
+    <t>amadeusivan</t>
+  </si>
+  <si>
+    <t>ongerijmd</t>
+  </si>
+  <si>
+    <t>umarebru</t>
+  </si>
+  <si>
+    <t>a_mieke</t>
+  </si>
+  <si>
+    <t>steephsel</t>
+  </si>
+  <si>
+    <t>brechtjedeleij</t>
+  </si>
+  <si>
+    <t>Opmerkingen</t>
+  </si>
+  <si>
+    <t>mix met en</t>
+  </si>
+  <si>
+    <t>eetschrijver</t>
+  </si>
+  <si>
+    <t>klapster</t>
+  </si>
+  <si>
+    <t>goedemorgenman</t>
+  </si>
+  <si>
+    <t>walterhoekstra</t>
+  </si>
+  <si>
+    <t>jasmijn02</t>
+  </si>
+  <si>
+    <t>miekeinc</t>
+  </si>
+  <si>
+    <t>sredlums</t>
+  </si>
+  <si>
+    <t>aldith_hunkar</t>
+  </si>
+  <si>
+    <t>tien020</t>
+  </si>
+  <si>
+    <t>karinwinters</t>
+  </si>
+  <si>
+    <t>johnschop</t>
+  </si>
+  <si>
+    <t>lobdozer</t>
+  </si>
+  <si>
+    <t>theollieworks</t>
+  </si>
+  <si>
+    <t>wup5</t>
+  </si>
+  <si>
+    <t>jennekepenneke</t>
+  </si>
+  <si>
+    <t>rebelsnotes</t>
+  </si>
+  <si>
+    <t>puberdochters</t>
+  </si>
+  <si>
+    <t>knotsbots</t>
+  </si>
+  <si>
+    <t>dennismons</t>
+  </si>
+  <si>
+    <t>fluist3r</t>
+  </si>
+  <si>
+    <t>mariannecramer</t>
+  </si>
+  <si>
+    <t>rjvanhouten</t>
+  </si>
+  <si>
+    <t>superjan</t>
+  </si>
+  <si>
+    <t>titchener</t>
+  </si>
+  <si>
+    <t>anniebbarks</t>
+  </si>
+  <si>
+    <t>fred3012</t>
+  </si>
+  <si>
+    <t>politicus1</t>
+  </si>
+  <si>
+    <t>peterstafleu</t>
+  </si>
+  <si>
+    <t>jettyvanrooy</t>
+  </si>
+  <si>
+    <t>mariannezw</t>
+  </si>
+  <si>
+    <t>jochemgeerdink</t>
+  </si>
+  <si>
+    <t>nabilfeki</t>
+  </si>
+  <si>
+    <t>kos_</t>
+  </si>
+  <si>
+    <t>esther_305</t>
+  </si>
+  <si>
+    <t>CKS COMMUNITY</t>
+  </si>
+  <si>
+    <t>SKSS COMMUNITY</t>
+  </si>
+  <si>
+    <t>SKKS OTHER</t>
+  </si>
+  <si>
+    <t>CKS OTHER</t>
   </si>
 </sst>
 </file>
@@ -2045,10 +2232,714 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>477584</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>36</v>
+      </c>
+      <c r="L2">
+        <v>33</v>
+      </c>
+      <c r="M2">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <v>324268</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>31</v>
+      </c>
+      <c r="H3">
+        <v>34</v>
+      </c>
+      <c r="L3">
+        <v>28</v>
+      </c>
+      <c r="M3">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>334816</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>35</v>
+      </c>
+      <c r="H4">
+        <v>39</v>
+      </c>
+      <c r="L4">
+        <v>33</v>
+      </c>
+      <c r="M4">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <v>297352</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>33</v>
+      </c>
+      <c r="G5">
+        <v>34</v>
+      </c>
+      <c r="H5">
+        <v>36</v>
+      </c>
+      <c r="L5">
+        <v>33</v>
+      </c>
+      <c r="M5">
+        <v>37</v>
+      </c>
+      <c r="N5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6">
+        <v>253684</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>36</v>
+      </c>
+      <c r="L6">
+        <v>30</v>
+      </c>
+      <c r="M6">
+        <v>36</v>
+      </c>
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7">
+        <v>291008</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>330960</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>316428</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10">
+        <v>286320</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>34</v>
+      </c>
+      <c r="F10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>272952</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12">
+        <v>258364</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>218380</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>26</v>
+      </c>
+      <c r="E13">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14">
+        <v>297144</v>
+      </c>
+      <c r="C14">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15">
+        <v>260072</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16">
+        <v>252460</v>
+      </c>
+      <c r="C16">
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17">
+        <v>201542</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18">
+        <v>276976</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19">
+        <v>256432</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>23</v>
+      </c>
+      <c r="F19">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20">
+        <v>249304</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24">
+        <v>21</v>
+      </c>
+      <c r="F24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25">
+        <v>25</v>
+      </c>
+      <c r="F25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2059,7 +2950,7 @@
     <col min="4" max="4" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2072,8 +2963,11 @@
       <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2084,7 +2978,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2095,7 +2989,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2108,8 +3002,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>55212868</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2123,7 +3020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -2140,12 +3037,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>